<commit_message>
front con opciones de listar proveedores, agregar nuevos, listar pedidos
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -1,59 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
-    <sheet sheetId="1" name="Pedidos" state="visible" r:id="rId4"/>
+    <sheet name="Pedidos" sheetId="1" r:id="rId1"/>
+    <sheet name="PINI" sheetId="2" r:id="rId2"/>
+    <sheet name="ooo" sheetId="3" r:id="rId3"/>
+    <sheet name="megatronic" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>Proveedor</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>agua</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>baba</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,21 +68,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -416,67 +399,167 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Proveedor</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Cantidad</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>a</v>
+      </c>
+      <c r="C2" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="str">
+        <v>agua</v>
+      </c>
+      <c r="C3" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>5</v>
+      </c>
+      <c r="B4" t="str">
+        <v>baba</v>
+      </c>
+      <c r="C4" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <v>b</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2</v>
+      </c>
+      <c r="C6" t="str">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Cantidad</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>MASO</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Cantidad</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Cantidad</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Readme.md con informacion sobre el proyecto(en desarrollo), funcionalidades completas funcionando, pequeño bug al eliminar el ultimo proveedor.
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -3,10 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
-    <sheet name="Pedidos" sheetId="1" r:id="rId1"/>
+    <sheet name="papa" sheetId="1" r:id="rId1"/>
     <sheet name="PINI" sheetId="2" r:id="rId2"/>
-    <sheet name="ooo" sheetId="3" r:id="rId3"/>
-    <sheet name="megatronic" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -400,98 +398,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Proveedor</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Producto</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Cantidad</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>a</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <v>agua</v>
-      </c>
-      <c r="C3" t="str">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>5</v>
-      </c>
-      <c r="B4" t="str">
-        <v>baba</v>
-      </c>
-      <c r="C4" t="str">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>b</v>
-      </c>
-      <c r="C5" t="str">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2</v>
-      </c>
-      <c r="C6" t="str">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -507,10 +413,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>MASO</v>
+        <v>Auricular Inalambrico</v>
       </c>
       <c r="B2" t="str">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -540,26 +446,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Producto</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Cantidad</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add estilos boostrap, imagen arquitectura
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="papa" sheetId="1" r:id="rId1"/>
     <sheet name="PINI" sheetId="2" r:id="rId2"/>
+    <sheet name="hola" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -398,6 +399,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Cantidad</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -413,10 +436,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Auricular Inalambrico</v>
+        <v>MASO</v>
       </c>
       <c r="B2" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -426,7 +449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>

<commit_message>
se agregan mas estilos, navegacion tipo pestaña, rutas relativas para poder usar desde celular
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -3,9 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
-    <sheet name="papa" sheetId="1" r:id="rId1"/>
-    <sheet name="PINI" sheetId="2" r:id="rId2"/>
-    <sheet name="hola" sheetId="3" r:id="rId3"/>
+    <sheet name="PINI" sheetId="1" r:id="rId1"/>
+    <sheet name="Algo" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -399,28 +398,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Producto</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Cantidad</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -436,10 +413,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>MASO</v>
+        <v>Sabana</v>
       </c>
       <c r="B2" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>

<commit_message>
archivo .bat para poder iniciar sistema sin entorno
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -4,7 +4,6 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
     <sheet name="PINI" sheetId="1" r:id="rId1"/>
-    <sheet name="Algo" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -413,10 +412,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sabana</v>
+        <v>a</v>
       </c>
       <c r="B2" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -424,26 +423,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Producto</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Cantidad</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
modificacion de atributos de tabla en front y back para definir el tipo de datos que necesita el cliente (producto y codigo)
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -410,17 +410,9 @@
         <v>Cantidad</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>a</v>
-      </c>
-      <c r="B2" t="str">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agrego seccion avisos funcionando, misma logica, falta pulir ux
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
     <sheet name="PINI" sheetId="1" r:id="rId1"/>
+    <sheet name="JUANCITO" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -415,4 +416,26 @@
     <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Producto</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Codigo</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>